<commit_message>
Added additional cross checking functionality against reported key metrics
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/AAPL/annual/stock_price_data.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/AAPL/annual/stock_price_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>high</t>
   </si>
@@ -26,6 +26,78 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1989</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1990</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1991</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1992</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1993</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1994</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1995</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1996</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1997</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1998</t>
+  </si>
+  <si>
+    <t>AAPL-FY-1999</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2000</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2001</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2002</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2003</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2004</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2005</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2006</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2007</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2008</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2009</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2010</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2011</t>
+  </si>
+  <si>
+    <t>AAPL-FY-2012</t>
   </si>
   <si>
     <t>AAPL-FY-2013</t>
@@ -413,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,13 +515,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>25.93499946594238</v>
+        <v>0.4497770071029663</v>
       </c>
       <c r="C3">
-        <v>16.94321441650391</v>
+        <v>0.2433039993047714</v>
       </c>
       <c r="D3">
-        <v>20.90607998760573</v>
+        <v>0.354091441702275</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,13 +529,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>33.6349983215332</v>
+        <v>0.6540179848670959</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>0.2165179997682571</v>
       </c>
       <c r="D4">
-        <v>29.64994020955971</v>
+        <v>0.4320348132815626</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,13 +543,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>30.95499992370605</v>
+        <v>0.625</v>
       </c>
       <c r="C5">
-        <v>22.36750030517578</v>
+        <v>0.3705359995365143</v>
       </c>
       <c r="D5">
-        <v>26.19310755938648</v>
+        <v>0.4837598591808259</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,13 +557,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>41.23500061035156</v>
+        <v>0.5825889706611633</v>
       </c>
       <c r="C6">
-        <v>26.02000045776367</v>
+        <v>0.2098210006952286</v>
       </c>
       <c r="D6">
-        <v>34.14772453904152</v>
+        <v>0.4218617693002045</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,13 +571,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>57.41749954223633</v>
+        <v>0.34375</v>
       </c>
       <c r="C7">
-        <v>37.56000137329102</v>
+        <v>0.1964289993047714</v>
       </c>
       <c r="D7">
-        <v>45.58395429816379</v>
+        <v>0.2819552562924713</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,13 +585,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>58.36750030517578</v>
+        <v>0.4475449919700623</v>
       </c>
       <c r="C8">
-        <v>35.5</v>
+        <v>0.2901790142059326</v>
       </c>
       <c r="D8">
-        <v>48.00395001220703</v>
+        <v>0.3673780051961777</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -527,13 +599,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>137.9799957275391</v>
+        <v>0.3794640004634857</v>
       </c>
       <c r="C9">
-        <v>53.15250015258789</v>
+        <v>0.1428570002317429</v>
       </c>
       <c r="D9">
-        <v>80.69004953999918</v>
+        <v>0.2511022906927836</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -541,13 +613,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>157.2599945068359</v>
+        <v>0.2639510035514832</v>
       </c>
       <c r="C10">
-        <v>107.3199996948242</v>
+        <v>0.1138390004634857</v>
       </c>
       <c r="D10">
-        <v>131.0207171193157</v>
+        <v>0.1755720084858319</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -555,12 +627,348 @@
         <v>13</v>
       </c>
       <c r="B11">
+        <v>0.390625</v>
+      </c>
+      <c r="C11">
+        <v>0.1138390004634857</v>
+      </c>
+      <c r="D11">
+        <v>0.2294782953136471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0.7154020071029663</v>
+      </c>
+      <c r="C12">
+        <v>0.2544640004634857</v>
+      </c>
+      <c r="D12">
+        <v>0.3933011308785469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1.342633962631226</v>
+      </c>
+      <c r="C13">
+        <v>0.453125</v>
+      </c>
+      <c r="D13">
+        <v>0.9245598661760411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0.4842860102653503</v>
+      </c>
+      <c r="C14">
+        <v>0.2433039993047714</v>
+      </c>
+      <c r="D14">
+        <v>0.3565608266635462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.4673210084438324</v>
+      </c>
+      <c r="C15">
+        <v>0.2464289963245392</v>
+      </c>
+      <c r="D15">
+        <v>0.3620105781165727</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.4164290130138397</v>
+      </c>
+      <c r="C16">
+        <v>0.2271430045366287</v>
+      </c>
+      <c r="D16">
+        <v>0.299975082396986</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0.6941069960594177</v>
+      </c>
+      <c r="C17">
+        <v>0.34375</v>
+      </c>
+      <c r="D17">
+        <v>0.4770635803937912</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1.921785950660706</v>
+      </c>
+      <c r="C18">
+        <v>0.65767902135849</v>
+      </c>
+      <c r="D18">
+        <v>1.325498145014521</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>3.085714101791382</v>
+      </c>
+      <c r="C19">
+        <v>1.709643006324768</v>
+      </c>
+      <c r="D19">
+        <v>2.346522038802505</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>5.535714149475098</v>
+      </c>
+      <c r="C20">
+        <v>2.592856884002686</v>
+      </c>
+      <c r="D20">
+        <v>3.712232831001282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>7.248570919036865</v>
+      </c>
+      <c r="C21">
+        <v>4.122857093811035</v>
+      </c>
+      <c r="D21">
+        <v>5.841691822644724</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>6.746428966522217</v>
+      </c>
+      <c r="C22">
+        <v>2.792856931686401</v>
+      </c>
+      <c r="D22">
+        <v>4.284210282017985</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>10.48321437835693</v>
+      </c>
+      <c r="C23">
+        <v>6.45357084274292</v>
+      </c>
+      <c r="D23">
+        <v>8.192667900328617</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>15.10214328765869</v>
+      </c>
+      <c r="C24">
+        <v>9.821429252624512</v>
+      </c>
+      <c r="D24">
+        <v>12.21202808713156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>25.18107032775879</v>
+      </c>
+      <c r="C25">
+        <v>12.65142917633057</v>
+      </c>
+      <c r="D25">
+        <v>18.81095007807016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>24.16964340209961</v>
+      </c>
+      <c r="C26">
+        <v>13.75357055664062</v>
+      </c>
+      <c r="D26">
+        <v>17.2969492142459</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>25.93499946594238</v>
+      </c>
+      <c r="C27">
+        <v>16.94321441650391</v>
+      </c>
+      <c r="D27">
+        <v>20.90607998760573</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>33.6349983215332</v>
+      </c>
+      <c r="C28">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>29.64994020955971</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>30.95499992370605</v>
+      </c>
+      <c r="C29">
+        <v>22.36750030517578</v>
+      </c>
+      <c r="D29">
+        <v>26.19310755938648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>41.23500061035156</v>
+      </c>
+      <c r="C30">
+        <v>26.02000045776367</v>
+      </c>
+      <c r="D30">
+        <v>34.14772453904152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>57.41749954223633</v>
+      </c>
+      <c r="C31">
+        <v>37.56000137329102</v>
+      </c>
+      <c r="D31">
+        <v>45.58395429816379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>58.36750030517578</v>
+      </c>
+      <c r="C32">
+        <v>35.5</v>
+      </c>
+      <c r="D32">
+        <v>48.00395001220703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>137.9799957275391</v>
+      </c>
+      <c r="C33">
+        <v>53.15250015258789</v>
+      </c>
+      <c r="D33">
+        <v>80.69004953999918</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>157.2599945068359</v>
+      </c>
+      <c r="C34">
+        <v>107.3199996948242</v>
+      </c>
+      <c r="D34">
+        <v>131.0207171193157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
         <v>182.9400024414062</v>
       </c>
-      <c r="C11">
+      <c r="C35">
         <v>129.0399932861328</v>
       </c>
-      <c r="D11">
+      <c r="D35">
         <v>158.6180480713863</v>
       </c>
     </row>

</xml_diff>